<commit_message>
add gender property to distributer
</commit_message>
<xml_diff>
--- a/prototypes/E5_distributer_system.xlsx
+++ b/prototypes/E5_distributer_system.xlsx
@@ -109,42 +109,43 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>比经验值</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>前三名比佣金</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseUrl</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.0.115</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>问题</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>注册成功之后如果通过wecharNo
+,phoneNo 在Customer表中未找到对应的数据，
+是否将新客户的数据插入到Customer表中</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">{'phoneNo':'18300001234',
       'password':'yzw123456',
       'name':'Angelina Jolie',
       'nickName':'Angelina',
+      'gender':‘female',
       'birthday':'2000-01-01',
       'followedByStore.id':63,
      'wechatNo':'sfsfsojmn',
       'invitationCode':'aaaaa'
      }
 </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>比经验值</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>前三名比佣金</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>baseUrl</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.0.115</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>问题</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>注册成功之后如果通过wecharNo
-,phoneNo 在Customer表中未找到对应的数据，
-是否将新客户的数据插入到Customer表中</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -541,7 +542,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -556,10 +557,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
@@ -579,10 +580,10 @@
         <v>9</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="135" x14ac:dyDescent="0.15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="148.5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -593,10 +594,10 @@
         <v>12</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
@@ -672,7 +673,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.15">
@@ -683,7 +684,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
修改 uedit.all.js中"accept/*" 改为 accept="image/gif,image/jpeg,image/png,image/jpg,image/bmp" 使图片上传窗口迅速打开
</commit_message>
<xml_diff>
--- a/prototypes/E5_distributer_system.xlsx
+++ b/prototypes/E5_distributer_system.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="12990" windowHeight="10155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12990" windowHeight="10155"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="95">
   <si>
     <t>将余额转入订金账户，用来购买产品</t>
   </si>
@@ -411,12 +411,87 @@
     <t>课程券是什么东东</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>/api/tweet/save</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>api/tweetType/list</t>
+  </si>
+  <si>
+    <t>获取所有推文类型</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>data:[{id:推文类型Id, name: 推文类型名}...]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/tweet/list</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>int tweetTypeId  //推文类型Id 必须， 全部类型id =0 
+String title     //推文标题, 非必须 按标题模糊查询</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>保存推文
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>富文本编辑器使用ueditor)</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>String author  //作者 必须
+String title  //富文本标题 必须
+String digest //简介 必须 50字以内
+multiFile coverIcon //推文简介图片 必须
+int tweetTypeId //推文类型Id  必须
+String content  // 推文富文本内容 必须</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取推文</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>data:{id: 推文Id, 
+author:推文作者，
+title: 推文标题，
+digest: 推文简介,
+coverIconUrl: 推文简介图片相对Url,</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -473,6 +548,14 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -843,21 +926,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="46" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5" style="5" customWidth="1"/>
     <col min="3" max="3" width="12" style="5" customWidth="1"/>
     <col min="4" max="4" width="21.75" style="5" customWidth="1"/>
     <col min="5" max="5" width="56.5" style="6" customWidth="1"/>
-    <col min="6" max="6" width="255.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23" style="5" customWidth="1"/>
+    <col min="6" max="6" width="50.625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="18" style="5" customWidth="1"/>
     <col min="8" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
@@ -1133,7 +1217,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
         <v>79</v>
       </c>
@@ -1145,6 +1229,60 @@
       </c>
       <c r="E17" s="6" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="81" x14ac:dyDescent="0.15">
+      <c r="A19" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A20" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
完成 /api/message/list， /api/message/id/{id} 接口
</commit_message>
<xml_diff>
--- a/prototypes/E5_distributer_system.xlsx
+++ b/prototypes/E5_distributer_system.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="112">
   <si>
     <t>将余额转入订金账户，用来购买产品</t>
   </si>
@@ -420,9 +420,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>api/tweetType/list</t>
-  </si>
-  <si>
     <t>获取所有推文类型</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -527,12 +524,82 @@
 int tweetId         //推文Id 必须</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>api/tweetType/list</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取消息列表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/message/list</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>int receiverId      //接收者Id  必须</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>data:[{id: 消息Id,
+ date:消息发送日期,
+ status: 消息状态（未读或已读)
+ content: 消息文本内容}]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/message/id/{id}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>data:{id: 消息Id,
+ date:消息发送日期,
+ status: 消息状态（未读或已读)
+ content: 消息文本内容}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>获取消息
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>获取之后会将状态设置为已读)</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">int id    //消息Id 必须 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>放在路径上</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -592,6 +659,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="3"/>
@@ -967,11 +1042,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1274,24 +1349,24 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="81" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>82</v>
@@ -1303,7 +1378,7 @@
         <v>46</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>71</v>
@@ -1311,53 +1386,87 @@
     </row>
     <row r="20" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>90</v>
-      </c>
       <c r="F20" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E21" s="6" t="s">
+      <c r="F21" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="E22" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>103</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="54" x14ac:dyDescent="0.15">
+      <c r="A23" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="54" x14ac:dyDescent="0.15">
+      <c r="A24" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
修复 多 customerDao 实例
</commit_message>
<xml_diff>
--- a/prototypes/E5_distributer_system.xlsx
+++ b/prototypes/E5_distributer_system.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12990" windowHeight="10155"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="12990" windowHeight="10155"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="2" r:id="rId1"/>
@@ -1200,9 +1200,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
完成 分享推文记录 /api/tweet/share/list 接口
</commit_message>
<xml_diff>
--- a/prototypes/E5_distributer_system.xlsx
+++ b/prototypes/E5_distributer_system.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace3\yiwu\prototypes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23610" windowHeight="7650"/>
   </bookViews>
@@ -11,12 +16,11 @@
     <sheet name="Question" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:F9"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="150">
   <si>
     <t>将余额转入订金账户，用来购买产品</t>
   </si>
@@ -744,6 +748,32 @@
   </si>
   <si>
     <t>data: true(or false) //已注册返回true</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>分享推文记录</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/tweet/share/list</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>int sharerId   //推文分享者Id 必须 (我，一级客户，二级客户)
+int beneficiaryId        //经验收益者Id 必须 (我)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>data:{id:推文分享记录Id,
+sharer:分享者姓名,
+shareDate: 分享日期,
+tweetTitle: 分享的推文标题,
+tweetType: 分享的推文类型,
+exp: 分享该推文后,beneficiaryId收获的经验值</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1194,11 +1224,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:F5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1605,131 +1635,131 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="54" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="81" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="54" x14ac:dyDescent="0.15">
+      <c r="A25" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="54" x14ac:dyDescent="0.15">
-      <c r="A25" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A26" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="54" x14ac:dyDescent="0.15">
+      <c r="A26" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="135" x14ac:dyDescent="0.15">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="135" x14ac:dyDescent="0.15">
       <c r="A28" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="94.5" x14ac:dyDescent="0.15">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A31" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>93</v>
@@ -1737,41 +1767,58 @@
       <c r="E31" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="F31" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+        <v>129</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>137</v>
       </c>
       <c r="C33" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A34" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E34" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F34" s="5" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
完成 /api/distributer/registerRecords/subordinates /api/distributer/registerRecords/secondaries 接口
</commit_message>
<xml_diff>
--- a/prototypes/E5_distributer_system.xlsx
+++ b/prototypes/E5_distributer_system.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="161">
   <si>
     <t>将余额转入订金账户，用来购买产品</t>
   </si>
@@ -794,6 +794,34 @@
   </si>
   <si>
     <t>/api/tweet/share/list/subordinates</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取一级客户注册记录</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取二级客户注册记录</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/distributer/registerRecords/subordinates</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/distributer/registerRecords/secondaries</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>int distributerId  //分享者Id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>data:[{registerDate: 注册日期,
+memberId:会员Id,
+memberName 会员名,
+superDistributerName:上级分销者姓名,
+exp:本人获取到的经验值}]</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -876,7 +904,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -895,6 +923,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -908,7 +942,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -938,6 +972,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1244,17 +1284,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="40.5" style="5" customWidth="1"/>
+    <col min="2" max="2" width="48.5" style="5" customWidth="1"/>
     <col min="3" max="3" width="12" style="5" customWidth="1"/>
     <col min="4" max="4" width="21.75" style="5" customWidth="1"/>
     <col min="5" max="5" width="56.5" style="6" customWidth="1"/>
@@ -1400,46 +1440,46 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A9" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A10" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="A11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>42</v>
@@ -1447,73 +1487,73 @@
       <c r="E11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="F11" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.15">
+      <c r="A13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="5" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="A14" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>70</v>
@@ -1521,358 +1561,392 @@
     </row>
     <row r="16" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>63</v>
       </c>
       <c r="E17" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A18" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A19" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A18" s="5" t="s">
+    <row r="20" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A20" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19" s="5" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="81" x14ac:dyDescent="0.15">
-      <c r="A20" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A21" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>85</v>
       </c>
       <c r="E21" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="81" x14ac:dyDescent="0.15">
+      <c r="A22" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A23" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F23" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A22" s="5" t="s">
+    <row r="24" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A24" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F24" s="6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A23" s="5" t="s">
+    <row r="25" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A25" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="81" x14ac:dyDescent="0.15">
-      <c r="A24" s="5" t="s">
+    <row r="26" spans="1:6" ht="81" x14ac:dyDescent="0.15">
+      <c r="A26" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="81" x14ac:dyDescent="0.15">
-      <c r="A25" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="81" x14ac:dyDescent="0.15">
-      <c r="A26" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>147</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="54" x14ac:dyDescent="0.15">
-      <c r="A27" s="5" t="s">
+    <row r="27" spans="1:6" ht="81" x14ac:dyDescent="0.15">
+      <c r="A27" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="81" x14ac:dyDescent="0.15">
+      <c r="A28" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="54" x14ac:dyDescent="0.15">
+      <c r="A29" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="54" x14ac:dyDescent="0.15">
-      <c r="A28" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A29" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>115</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="135" x14ac:dyDescent="0.15">
-      <c r="A30" s="5" t="s">
-        <v>116</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="54" x14ac:dyDescent="0.15">
+      <c r="A30" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A31" s="5" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="94.5" x14ac:dyDescent="0.15">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="135" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="94.5" x14ac:dyDescent="0.15">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
+        <v>126</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E35" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A36" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A37" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="F37" s="6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A36" s="5" t="s">
+    <row r="38" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A38" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E38" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F38" s="5" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
完成BaseServiceImpl.modify(PK id, T entity)
</commit_message>
<xml_diff>
--- a/prototypes/E5_distributer_system.xlsx
+++ b/prototypes/E5_distributer_system.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="176">
   <si>
     <t>将余额转入订金账户，用来购买产品</t>
   </si>
@@ -899,6 +899,17 @@
 followedByStoreId://数据归属门店
 wechatNo://微信openId    必须
 invitationCode: //邀请码}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{name:
+nickName:
+phoneNo:
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>data{true or false}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1370,8 +1381,8 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1544,7 +1555,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A10" s="15" t="s">
         <v>167</v>
       </c>
@@ -1553,6 +1564,12 @@
       </c>
       <c r="C10" s="5" t="s">
         <v>169</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
修改 /api/order/{id} get 接口
</commit_message>
<xml_diff>
--- a/prototypes/E5_distributer_system.xlsx
+++ b/prototypes/E5_distributer_system.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="184">
   <si>
     <t>将余额转入订金账户，用来购买产品</t>
   </si>
@@ -595,27 +595,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>/api/order/id/{id}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>String id    //订单Id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>data:{id:订单Id,
-contractNo: 合同编号,
-productType: 产品类型（开放式，封闭式，私教课),
-validityTimes: 合约有效次数,
-contractStart: 合约开始时间,
-contractEnd: 合约结束时间,
-courseId: 课程Id,
-courseName: 课程名，
-courseStore:上课门店，
-courseStartDate: 课程开始日期}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>获取课程</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -943,11 +922,29 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>{eContractStatus:boolean}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>data:{true}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/order/{id}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>data:{id:订单Id,
+contractNo: 合同编号,
+productType: 产品类型（开放式，封闭式，私教课),
+validityTimes: 合约有效次数,
+contractStart: 合约开始时间,
+contractEnd: 合约结束时间,
+courseId: 课程Id,
+courseName: 课程名，
+courseStore:上课门店，
+courseStartDate: 课程开始日期,
+eContractStatus: 订单的确认状态(true,false)}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{eContractStatus:boolean (0,1,'true','false')}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1428,8 +1425,8 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1486,10 +1483,10 @@
         <v>12</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>25</v>
@@ -1497,37 +1494,37 @@
     </row>
     <row r="4" spans="1:7" ht="189.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>170</v>
-      </c>
       <c r="F4" s="12" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>135</v>
-      </c>
       <c r="C5" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>133</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>136</v>
       </c>
       <c r="G5" s="6"/>
     </row>
@@ -1545,7 +1542,7 @@
         <v>28</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="195" x14ac:dyDescent="0.15">
@@ -1562,7 +1559,7 @@
         <v>20</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.15">
@@ -1604,53 +1601,53 @@
     </row>
     <row r="10" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A10" s="15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A11" s="13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A12" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>151</v>
-      </c>
       <c r="F12" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
@@ -1715,7 +1712,7 @@
         <v>40</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>55</v>
@@ -1723,10 +1720,10 @@
     </row>
     <row r="17" spans="1:6" ht="81" x14ac:dyDescent="0.15">
       <c r="A17" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>156</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>40</v>
@@ -1735,15 +1732,15 @@
         <v>42</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="81" x14ac:dyDescent="0.15">
       <c r="A18" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>157</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>40</v>
@@ -1752,7 +1749,7 @@
         <v>42</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
@@ -1854,7 +1851,7 @@
         <v>77</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
@@ -1947,53 +1944,53 @@
     </row>
     <row r="30" spans="1:6" ht="81" x14ac:dyDescent="0.15">
       <c r="A30" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E30" s="6" t="s">
+      <c r="F30" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="81" x14ac:dyDescent="0.15">
       <c r="A31" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>142</v>
-      </c>
       <c r="F31" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="81" x14ac:dyDescent="0.15">
       <c r="A32" s="14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C32" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>142</v>
-      </c>
       <c r="F32" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="54" x14ac:dyDescent="0.15">
@@ -2047,137 +2044,134 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="135" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="148.5" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
         <v>113</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>114</v>
+        <v>181</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>115</v>
-      </c>
       <c r="F36" s="6" t="s">
-        <v>116</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" s="15" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>183</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A38" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>90</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>90</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A40" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>90</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>90</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A42" s="15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>90</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="54" x14ac:dyDescent="0.15">
       <c r="A43" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>171</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2202,10 +2196,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>